<commit_message>
template filtering, highlightin of mandatory of mandatory columns added
</commit_message>
<xml_diff>
--- a/schema_definitions/association_schema.xlsx
+++ b/schema_definitions/association_schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Project/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4357F96-1D17-FB49-BF57-838118CD51C3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFF13E0-A32B-4444-A6BC-2FD7A26FC643}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36400" yWindow="3480" windowWidth="27240" windowHeight="16040" xr2:uid="{22711B0A-61A0-604C-9980-93A48F0A9B95}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{22711B0A-61A0-604C-9980-93A48F0A9B95}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>standard_error</t>
+  </si>
+  <si>
+    <t>DEFAULT</t>
   </si>
 </sst>
 </file>
@@ -571,22 +574,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7DB89A1-2EB9-5B47-B02D-143094DA390C}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="66.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -594,34 +600,37 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>43</v>
       </c>
@@ -631,22 +640,25 @@
       <c r="C2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="1"/>
+      <c r="J2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
@@ -656,22 +668,25 @@
       <c r="C3" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="1"/>
+      <c r="J3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K3" s="1"/>
+      <c r="L3" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>45</v>
       </c>
@@ -681,22 +696,25 @@
       <c r="C4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="1"/>
+      <c r="J4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K4" s="1"/>
+      <c r="L4" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>46</v>
       </c>
@@ -706,26 +724,29 @@
       <c r="C5" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K5" s="1"/>
+      <c r="L5" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
@@ -733,24 +754,27 @@
         <v>19</v>
       </c>
       <c r="C6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="1"/>
+      <c r="J6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K6" s="1"/>
+      <c r="L6" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>48</v>
       </c>
@@ -760,22 +784,25 @@
       <c r="C7" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="1"/>
+      <c r="J7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K7" s="1"/>
+      <c r="L7" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>49</v>
       </c>
@@ -785,22 +812,25 @@
       <c r="C8" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="1"/>
+      <c r="J8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>50</v>
       </c>
@@ -808,24 +838,27 @@
         <v>26</v>
       </c>
       <c r="C9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="1"/>
+      <c r="J9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
@@ -835,20 +868,23 @@
       <c r="C10" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="1"/>
+      <c r="J10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>52</v>
       </c>
@@ -858,20 +894,23 @@
       <c r="C11" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="1"/>
+      <c r="J11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>53</v>
       </c>
@@ -881,20 +920,23 @@
       <c r="C12" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="1"/>
+      <c r="J12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
@@ -904,20 +946,23 @@
       <c r="C13" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="1" t="s">
+      <c r="I13" s="1"/>
+      <c r="J13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
@@ -927,20 +972,23 @@
       <c r="C14" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="1" t="s">
+      <c r="I14" s="1"/>
+      <c r="J14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>56</v>
       </c>
@@ -950,20 +998,23 @@
       <c r="C15" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="1" t="s">
+      <c r="I15" s="1"/>
+      <c r="J15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>57</v>
       </c>
@@ -973,18 +1024,21 @@
       <c r="C16" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="1"/>
+      <c r="J16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J16" s="1"/>
       <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>